<commit_message>
Edit rules tts in dict.py
</commit_message>
<xml_diff>
--- a/it_dict.xlsx
+++ b/it_dict.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="133">
   <si>
     <t xml:space="preserve">word</t>
   </si>
@@ -58,10 +58,13 @@
     <t xml:space="preserve">ip</t>
   </si>
   <si>
-    <t xml:space="preserve">уникальный адрес компьютера в Сети</t>
-  </si>
-  <si>
-    <t xml:space="preserve">уникальный адрес компьютера в Сети, который присваивается провайдером индивидуально каждому устройству и даёт возможность выхода в Интернет</t>
+    <t xml:space="preserve">уникальный адрес компьютера в cети</t>
+  </si>
+  <si>
+    <t xml:space="preserve">уникальный адрес компьютера в cети, который присваивается провайдером индивидуально каждому устройству и даёт возможность выхода в интернет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">уникальный адрес компьютера в сети</t>
   </si>
   <si>
     <t xml:space="preserve">апи</t>
@@ -504,7 +507,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -537,14 +540,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -569,13 +564,13 @@
   <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="30.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.55"/>
@@ -634,551 +629,551 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
     <row r="6" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" s="6" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
     <row r="20" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" s="7" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
     <row r="25" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
     <row r="26" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
     <row r="27" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" s="9" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B29" s="8" t="s">
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="B29" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="C29" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
+      <c r="D29" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="10"/>
+      <c r="C38" s="8"/>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="10"/>
+      <c r="C39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="10"/>
+      <c r="C40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="10"/>
+      <c r="C41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="10"/>
+      <c r="C42" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="10"/>
+      <c r="C43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="10"/>
+      <c r="C44" s="8"/>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="10"/>
+      <c r="C45" s="8"/>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="10"/>
+      <c r="C46" s="8"/>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="10"/>
+      <c r="C47" s="8"/>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="10"/>
+      <c r="C48" s="8"/>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="10"/>
+      <c r="C49" s="8"/>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="10"/>
+      <c r="C50" s="8"/>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="10"/>
+      <c r="C51" s="8"/>
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="10"/>
+      <c r="C52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="10"/>
+      <c r="C53" s="8"/>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="10"/>
+      <c r="C54" s="8"/>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="10"/>
+      <c r="C55" s="8"/>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="10"/>
+      <c r="C56" s="8"/>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="10"/>
+      <c r="C57" s="8"/>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="10"/>
+      <c r="C58" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>